<commit_message>
Updated to 2023 data. Added header argument to download.file function
</commit_message>
<xml_diff>
--- a/data/cpi.xlsx
+++ b/data/cpi.xlsx
@@ -17,89 +17,89 @@
     <sheet name="Enquiries" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="A2325806K">Data1!$B$1:$B$10,Data1!$B$11:$B$311</definedName>
-    <definedName name="A2325806K_Data">Data1!$B$11:$B$311</definedName>
-    <definedName name="A2325806K_Latest">Data1!$B$311</definedName>
-    <definedName name="A2325807L">Data1!$K$1:$K$10,Data1!$K$15:$K$311</definedName>
-    <definedName name="A2325807L_Data">Data1!$K$15:$K$311</definedName>
-    <definedName name="A2325807L_Latest">Data1!$K$311</definedName>
-    <definedName name="A2325810A">Data1!$T$1:$T$10,Data1!$T$12:$T$311</definedName>
-    <definedName name="A2325810A_Data">Data1!$T$12:$T$311</definedName>
-    <definedName name="A2325810A_Latest">Data1!$T$311</definedName>
-    <definedName name="A2325811C">Data1!$C$1:$C$10,Data1!$C$11:$C$311</definedName>
-    <definedName name="A2325811C_Data">Data1!$C$11:$C$311</definedName>
-    <definedName name="A2325811C_Latest">Data1!$C$311</definedName>
-    <definedName name="A2325812F">Data1!$L$1:$L$10,Data1!$L$15:$L$311</definedName>
-    <definedName name="A2325812F_Data">Data1!$L$15:$L$311</definedName>
-    <definedName name="A2325812F_Latest">Data1!$L$311</definedName>
-    <definedName name="A2325815L">Data1!$U$1:$U$10,Data1!$U$12:$U$311</definedName>
-    <definedName name="A2325815L_Data">Data1!$U$12:$U$311</definedName>
-    <definedName name="A2325815L_Latest">Data1!$U$311</definedName>
-    <definedName name="A2325816R">Data1!$D$1:$D$10,Data1!$D$11:$D$311</definedName>
-    <definedName name="A2325816R_Data">Data1!$D$11:$D$311</definedName>
-    <definedName name="A2325816R_Latest">Data1!$D$311</definedName>
-    <definedName name="A2325817T">Data1!$M$1:$M$10,Data1!$M$15:$M$311</definedName>
-    <definedName name="A2325817T_Data">Data1!$M$15:$M$311</definedName>
-    <definedName name="A2325817T_Latest">Data1!$M$311</definedName>
-    <definedName name="A2325820F">Data1!$V$1:$V$10,Data1!$V$12:$V$311</definedName>
-    <definedName name="A2325820F_Data">Data1!$V$12:$V$311</definedName>
-    <definedName name="A2325820F_Latest">Data1!$V$311</definedName>
-    <definedName name="A2325821J">Data1!$E$1:$E$10,Data1!$E$11:$E$311</definedName>
-    <definedName name="A2325821J_Data">Data1!$E$11:$E$311</definedName>
-    <definedName name="A2325821J_Latest">Data1!$E$311</definedName>
-    <definedName name="A2325822K">Data1!$N$1:$N$10,Data1!$N$15:$N$311</definedName>
-    <definedName name="A2325822K_Data">Data1!$N$15:$N$311</definedName>
-    <definedName name="A2325822K_Latest">Data1!$N$311</definedName>
-    <definedName name="A2325825T">Data1!$W$1:$W$10,Data1!$W$12:$W$311</definedName>
-    <definedName name="A2325825T_Data">Data1!$W$12:$W$311</definedName>
-    <definedName name="A2325825T_Latest">Data1!$W$311</definedName>
-    <definedName name="A2325826V">Data1!$F$1:$F$10,Data1!$F$11:$F$311</definedName>
-    <definedName name="A2325826V_Data">Data1!$F$11:$F$311</definedName>
-    <definedName name="A2325826V_Latest">Data1!$F$311</definedName>
-    <definedName name="A2325827W">Data1!$O$1:$O$10,Data1!$O$15:$O$311</definedName>
-    <definedName name="A2325827W_Data">Data1!$O$15:$O$311</definedName>
-    <definedName name="A2325827W_Latest">Data1!$O$311</definedName>
-    <definedName name="A2325830K">Data1!$X$1:$X$10,Data1!$X$12:$X$311</definedName>
-    <definedName name="A2325830K_Data">Data1!$X$12:$X$311</definedName>
-    <definedName name="A2325830K_Latest">Data1!$X$311</definedName>
-    <definedName name="A2325831L">Data1!$G$1:$G$10,Data1!$G$11:$G$311</definedName>
-    <definedName name="A2325831L_Data">Data1!$G$11:$G$311</definedName>
-    <definedName name="A2325831L_Latest">Data1!$G$311</definedName>
-    <definedName name="A2325832R">Data1!$P$1:$P$10,Data1!$P$15:$P$311</definedName>
-    <definedName name="A2325832R_Data">Data1!$P$15:$P$311</definedName>
-    <definedName name="A2325832R_Latest">Data1!$P$311</definedName>
-    <definedName name="A2325835W">Data1!$Y$1:$Y$10,Data1!$Y$12:$Y$311</definedName>
-    <definedName name="A2325835W_Data">Data1!$Y$12:$Y$311</definedName>
-    <definedName name="A2325835W_Latest">Data1!$Y$311</definedName>
-    <definedName name="A2325836X">Data1!$H$1:$H$10,Data1!$H$139:$H$311</definedName>
-    <definedName name="A2325836X_Data">Data1!$H$139:$H$311</definedName>
-    <definedName name="A2325836X_Latest">Data1!$H$311</definedName>
-    <definedName name="A2325837A">Data1!$Q$1:$Q$10,Data1!$Q$143:$Q$311</definedName>
-    <definedName name="A2325837A_Data">Data1!$Q$143:$Q$311</definedName>
-    <definedName name="A2325837A_Latest">Data1!$Q$311</definedName>
-    <definedName name="A2325840R">Data1!$Z$1:$Z$10,Data1!$Z$140:$Z$311</definedName>
-    <definedName name="A2325840R_Data">Data1!$Z$140:$Z$311</definedName>
-    <definedName name="A2325840R_Latest">Data1!$Z$311</definedName>
-    <definedName name="A2325841T">Data1!$I$1:$I$10,Data1!$I$11:$I$311</definedName>
-    <definedName name="A2325841T_Data">Data1!$I$11:$I$311</definedName>
-    <definedName name="A2325841T_Latest">Data1!$I$311</definedName>
-    <definedName name="A2325842V">Data1!$R$1:$R$10,Data1!$R$15:$R$311</definedName>
-    <definedName name="A2325842V_Data">Data1!$R$15:$R$311</definedName>
-    <definedName name="A2325842V_Latest">Data1!$R$311</definedName>
-    <definedName name="A2325845A">Data1!$AA$1:$AA$10,Data1!$AA$12:$AA$311</definedName>
-    <definedName name="A2325845A_Data">Data1!$AA$12:$AA$311</definedName>
-    <definedName name="A2325845A_Latest">Data1!$AA$311</definedName>
-    <definedName name="A2325846C">Data1!$J$1:$J$10,Data1!$J$11:$J$311</definedName>
-    <definedName name="A2325846C_Data">Data1!$J$11:$J$311</definedName>
-    <definedName name="A2325846C_Latest">Data1!$J$311</definedName>
-    <definedName name="A2325847F">Data1!$S$1:$S$10,Data1!$S$15:$S$311</definedName>
-    <definedName name="A2325847F_Data">Data1!$S$15:$S$311</definedName>
-    <definedName name="A2325847F_Latest">Data1!$S$311</definedName>
-    <definedName name="A2325850V">Data1!$AB$1:$AB$10,Data1!$AB$12:$AB$311</definedName>
-    <definedName name="A2325850V_Data">Data1!$AB$12:$AB$311</definedName>
-    <definedName name="A2325850V_Latest">Data1!$AB$311</definedName>
-    <definedName name="Date_Range">Data1!$A$2:$A$10,Data1!$A$11:$A$311</definedName>
-    <definedName name="Date_Range_Data">Data1!$A$11:$A$311</definedName>
+    <definedName name="A2325806K">Data1!$B$1:$B$10,Data1!$B$11:$B$312</definedName>
+    <definedName name="A2325806K_Data">Data1!$B$11:$B$312</definedName>
+    <definedName name="A2325806K_Latest">Data1!$B$312</definedName>
+    <definedName name="A2325807L">Data1!$K$1:$K$10,Data1!$K$15:$K$312</definedName>
+    <definedName name="A2325807L_Data">Data1!$K$15:$K$312</definedName>
+    <definedName name="A2325807L_Latest">Data1!$K$312</definedName>
+    <definedName name="A2325810A">Data1!$T$1:$T$10,Data1!$T$12:$T$312</definedName>
+    <definedName name="A2325810A_Data">Data1!$T$12:$T$312</definedName>
+    <definedName name="A2325810A_Latest">Data1!$T$312</definedName>
+    <definedName name="A2325811C">Data1!$C$1:$C$10,Data1!$C$11:$C$312</definedName>
+    <definedName name="A2325811C_Data">Data1!$C$11:$C$312</definedName>
+    <definedName name="A2325811C_Latest">Data1!$C$312</definedName>
+    <definedName name="A2325812F">Data1!$L$1:$L$10,Data1!$L$15:$L$312</definedName>
+    <definedName name="A2325812F_Data">Data1!$L$15:$L$312</definedName>
+    <definedName name="A2325812F_Latest">Data1!$L$312</definedName>
+    <definedName name="A2325815L">Data1!$U$1:$U$10,Data1!$U$12:$U$312</definedName>
+    <definedName name="A2325815L_Data">Data1!$U$12:$U$312</definedName>
+    <definedName name="A2325815L_Latest">Data1!$U$312</definedName>
+    <definedName name="A2325816R">Data1!$D$1:$D$10,Data1!$D$11:$D$312</definedName>
+    <definedName name="A2325816R_Data">Data1!$D$11:$D$312</definedName>
+    <definedName name="A2325816R_Latest">Data1!$D$312</definedName>
+    <definedName name="A2325817T">Data1!$M$1:$M$10,Data1!$M$15:$M$312</definedName>
+    <definedName name="A2325817T_Data">Data1!$M$15:$M$312</definedName>
+    <definedName name="A2325817T_Latest">Data1!$M$312</definedName>
+    <definedName name="A2325820F">Data1!$V$1:$V$10,Data1!$V$12:$V$312</definedName>
+    <definedName name="A2325820F_Data">Data1!$V$12:$V$312</definedName>
+    <definedName name="A2325820F_Latest">Data1!$V$312</definedName>
+    <definedName name="A2325821J">Data1!$E$1:$E$10,Data1!$E$11:$E$312</definedName>
+    <definedName name="A2325821J_Data">Data1!$E$11:$E$312</definedName>
+    <definedName name="A2325821J_Latest">Data1!$E$312</definedName>
+    <definedName name="A2325822K">Data1!$N$1:$N$10,Data1!$N$15:$N$312</definedName>
+    <definedName name="A2325822K_Data">Data1!$N$15:$N$312</definedName>
+    <definedName name="A2325822K_Latest">Data1!$N$312</definedName>
+    <definedName name="A2325825T">Data1!$W$1:$W$10,Data1!$W$12:$W$312</definedName>
+    <definedName name="A2325825T_Data">Data1!$W$12:$W$312</definedName>
+    <definedName name="A2325825T_Latest">Data1!$W$312</definedName>
+    <definedName name="A2325826V">Data1!$F$1:$F$10,Data1!$F$11:$F$312</definedName>
+    <definedName name="A2325826V_Data">Data1!$F$11:$F$312</definedName>
+    <definedName name="A2325826V_Latest">Data1!$F$312</definedName>
+    <definedName name="A2325827W">Data1!$O$1:$O$10,Data1!$O$15:$O$312</definedName>
+    <definedName name="A2325827W_Data">Data1!$O$15:$O$312</definedName>
+    <definedName name="A2325827W_Latest">Data1!$O$312</definedName>
+    <definedName name="A2325830K">Data1!$X$1:$X$10,Data1!$X$12:$X$312</definedName>
+    <definedName name="A2325830K_Data">Data1!$X$12:$X$312</definedName>
+    <definedName name="A2325830K_Latest">Data1!$X$312</definedName>
+    <definedName name="A2325831L">Data1!$G$1:$G$10,Data1!$G$11:$G$312</definedName>
+    <definedName name="A2325831L_Data">Data1!$G$11:$G$312</definedName>
+    <definedName name="A2325831L_Latest">Data1!$G$312</definedName>
+    <definedName name="A2325832R">Data1!$P$1:$P$10,Data1!$P$15:$P$312</definedName>
+    <definedName name="A2325832R_Data">Data1!$P$15:$P$312</definedName>
+    <definedName name="A2325832R_Latest">Data1!$P$312</definedName>
+    <definedName name="A2325835W">Data1!$Y$1:$Y$10,Data1!$Y$12:$Y$312</definedName>
+    <definedName name="A2325835W_Data">Data1!$Y$12:$Y$312</definedName>
+    <definedName name="A2325835W_Latest">Data1!$Y$312</definedName>
+    <definedName name="A2325836X">Data1!$H$1:$H$10,Data1!$H$139:$H$312</definedName>
+    <definedName name="A2325836X_Data">Data1!$H$139:$H$312</definedName>
+    <definedName name="A2325836X_Latest">Data1!$H$312</definedName>
+    <definedName name="A2325837A">Data1!$Q$1:$Q$10,Data1!$Q$143:$Q$312</definedName>
+    <definedName name="A2325837A_Data">Data1!$Q$143:$Q$312</definedName>
+    <definedName name="A2325837A_Latest">Data1!$Q$312</definedName>
+    <definedName name="A2325840R">Data1!$Z$1:$Z$10,Data1!$Z$140:$Z$312</definedName>
+    <definedName name="A2325840R_Data">Data1!$Z$140:$Z$312</definedName>
+    <definedName name="A2325840R_Latest">Data1!$Z$312</definedName>
+    <definedName name="A2325841T">Data1!$I$1:$I$10,Data1!$I$11:$I$312</definedName>
+    <definedName name="A2325841T_Data">Data1!$I$11:$I$312</definedName>
+    <definedName name="A2325841T_Latest">Data1!$I$312</definedName>
+    <definedName name="A2325842V">Data1!$R$1:$R$10,Data1!$R$15:$R$312</definedName>
+    <definedName name="A2325842V_Data">Data1!$R$15:$R$312</definedName>
+    <definedName name="A2325842V_Latest">Data1!$R$312</definedName>
+    <definedName name="A2325845A">Data1!$AA$1:$AA$10,Data1!$AA$12:$AA$312</definedName>
+    <definedName name="A2325845A_Data">Data1!$AA$12:$AA$312</definedName>
+    <definedName name="A2325845A_Latest">Data1!$AA$312</definedName>
+    <definedName name="A2325846C">Data1!$J$1:$J$10,Data1!$J$11:$J$312</definedName>
+    <definedName name="A2325846C_Data">Data1!$J$11:$J$312</definedName>
+    <definedName name="A2325846C_Latest">Data1!$J$312</definedName>
+    <definedName name="A2325847F">Data1!$S$1:$S$10,Data1!$S$15:$S$312</definedName>
+    <definedName name="A2325847F_Data">Data1!$S$15:$S$312</definedName>
+    <definedName name="A2325847F_Latest">Data1!$S$312</definedName>
+    <definedName name="A2325850V">Data1!$AB$1:$AB$10,Data1!$AB$12:$AB$312</definedName>
+    <definedName name="A2325850V_Data">Data1!$AB$12:$AB$312</definedName>
+    <definedName name="A2325850V_Latest">Data1!$AB$312</definedName>
+    <definedName name="Date_Range">Data1!$A$2:$A$10,Data1!$A$11:$A$312</definedName>
+    <definedName name="Date_Range_Data">Data1!$A$11:$A$312</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -629,7 +629,7 @@
     <t>Freq.</t>
   </si>
   <si>
-    <t>© Commonwealth of Australia  2023</t>
+    <t>© Commonwealth of Australia  2024</t>
   </si>
 </sst>
 </file>
@@ -1316,10 +1316,10 @@
         <v>17777</v>
       </c>
       <c r="G12" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H12" s="10">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>36</v>
@@ -1348,10 +1348,10 @@
         <v>17777</v>
       </c>
       <c r="G13" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H13" s="10">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>36</v>
@@ -1380,10 +1380,10 @@
         <v>17777</v>
       </c>
       <c r="G14" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H14" s="10">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>36</v>
@@ -1412,10 +1412,10 @@
         <v>17777</v>
       </c>
       <c r="G15" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H15" s="10">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>36</v>
@@ -1444,10 +1444,10 @@
         <v>17777</v>
       </c>
       <c r="G16" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H16" s="10">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>36</v>
@@ -1476,10 +1476,10 @@
         <v>17777</v>
       </c>
       <c r="G17" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H17" s="10">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>36</v>
@@ -1508,10 +1508,10 @@
         <v>29465</v>
       </c>
       <c r="G18" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H18" s="10">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>36</v>
@@ -1540,10 +1540,10 @@
         <v>17777</v>
       </c>
       <c r="G19" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H19" s="10">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>36</v>
@@ -1572,10 +1572,10 @@
         <v>17777</v>
       </c>
       <c r="G20" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H20" s="10">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>36</v>
@@ -1604,10 +1604,10 @@
         <v>18142</v>
       </c>
       <c r="G21" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H21" s="10">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>49</v>
@@ -1636,10 +1636,10 @@
         <v>18142</v>
       </c>
       <c r="G22" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H22" s="10">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>49</v>
@@ -1668,10 +1668,10 @@
         <v>18142</v>
       </c>
       <c r="G23" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H23" s="10">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>49</v>
@@ -1700,10 +1700,10 @@
         <v>18142</v>
       </c>
       <c r="G24" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H24" s="10">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>49</v>
@@ -1732,10 +1732,10 @@
         <v>18142</v>
       </c>
       <c r="G25" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H25" s="10">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>49</v>
@@ -1764,10 +1764,10 @@
         <v>18142</v>
       </c>
       <c r="G26" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H26" s="10">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>49</v>
@@ -1796,10 +1796,10 @@
         <v>29830</v>
       </c>
       <c r="G27" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H27" s="10">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>49</v>
@@ -1828,10 +1828,10 @@
         <v>18142</v>
       </c>
       <c r="G28" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H28" s="10">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>49</v>
@@ -1860,10 +1860,10 @@
         <v>18142</v>
       </c>
       <c r="G29" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H29" s="10">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>49</v>
@@ -1892,10 +1892,10 @@
         <v>17868</v>
       </c>
       <c r="G30" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H30" s="10">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>49</v>
@@ -1924,10 +1924,10 @@
         <v>17868</v>
       </c>
       <c r="G31" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H31" s="10">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>49</v>
@@ -1956,10 +1956,10 @@
         <v>17868</v>
       </c>
       <c r="G32" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H32" s="10">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>49</v>
@@ -1988,10 +1988,10 @@
         <v>17868</v>
       </c>
       <c r="G33" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H33" s="10">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>49</v>
@@ -2020,10 +2020,10 @@
         <v>17868</v>
       </c>
       <c r="G34" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H34" s="10">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>49</v>
@@ -2052,10 +2052,10 @@
         <v>17868</v>
       </c>
       <c r="G35" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H35" s="10">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>49</v>
@@ -2084,10 +2084,10 @@
         <v>29556</v>
       </c>
       <c r="G36" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H36" s="10">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I36" s="10" t="s">
         <v>49</v>
@@ -2116,10 +2116,10 @@
         <v>17868</v>
       </c>
       <c r="G37" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H37" s="10">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I37" s="10" t="s">
         <v>49</v>
@@ -2148,10 +2148,10 @@
         <v>17868</v>
       </c>
       <c r="G38" s="9">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H38" s="10">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>49</v>
@@ -2213,7 +2213,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB311"/>
+  <dimension ref="A1:AB312"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
@@ -2831,85 +2831,85 @@
         <v>33</v>
       </c>
       <c r="B8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="C8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="D8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="E8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="F8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="G8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="H8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="I8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="J8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="K8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="L8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="M8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="N8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="O8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="P8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="Q8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="R8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="S8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="T8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="U8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="V8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="W8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="X8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="Y8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="Z8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="AA8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
       <c r="AB8" s="6">
-        <v>45170</v>
+        <v>45261</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
@@ -2917,85 +2917,85 @@
         <v>34</v>
       </c>
       <c r="B9" s="1">
+        <v>302</v>
+      </c>
+      <c r="C9" s="1">
+        <v>302</v>
+      </c>
+      <c r="D9" s="1">
+        <v>302</v>
+      </c>
+      <c r="E9" s="1">
+        <v>302</v>
+      </c>
+      <c r="F9" s="1">
+        <v>302</v>
+      </c>
+      <c r="G9" s="1">
+        <v>302</v>
+      </c>
+      <c r="H9" s="1">
+        <v>174</v>
+      </c>
+      <c r="I9" s="1">
+        <v>302</v>
+      </c>
+      <c r="J9" s="1">
+        <v>302</v>
+      </c>
+      <c r="K9" s="1">
+        <v>298</v>
+      </c>
+      <c r="L9" s="1">
+        <v>298</v>
+      </c>
+      <c r="M9" s="1">
+        <v>298</v>
+      </c>
+      <c r="N9" s="1">
+        <v>298</v>
+      </c>
+      <c r="O9" s="1">
+        <v>298</v>
+      </c>
+      <c r="P9" s="1">
+        <v>298</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>170</v>
+      </c>
+      <c r="R9" s="1">
+        <v>298</v>
+      </c>
+      <c r="S9" s="1">
+        <v>298</v>
+      </c>
+      <c r="T9" s="1">
         <v>301</v>
       </c>
-      <c r="C9" s="1">
+      <c r="U9" s="1">
         <v>301</v>
       </c>
-      <c r="D9" s="1">
+      <c r="V9" s="1">
         <v>301</v>
       </c>
-      <c r="E9" s="1">
+      <c r="W9" s="1">
         <v>301</v>
       </c>
-      <c r="F9" s="1">
+      <c r="X9" s="1">
         <v>301</v>
       </c>
-      <c r="G9" s="1">
+      <c r="Y9" s="1">
         <v>301</v>
       </c>
-      <c r="H9" s="1">
+      <c r="Z9" s="1">
         <v>173</v>
       </c>
-      <c r="I9" s="1">
+      <c r="AA9" s="1">
         <v>301</v>
       </c>
-      <c r="J9" s="1">
+      <c r="AB9" s="1">
         <v>301</v>
-      </c>
-      <c r="K9" s="1">
-        <v>297</v>
-      </c>
-      <c r="L9" s="1">
-        <v>297</v>
-      </c>
-      <c r="M9" s="1">
-        <v>297</v>
-      </c>
-      <c r="N9" s="1">
-        <v>297</v>
-      </c>
-      <c r="O9" s="1">
-        <v>297</v>
-      </c>
-      <c r="P9" s="1">
-        <v>297</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>169</v>
-      </c>
-      <c r="R9" s="1">
-        <v>297</v>
-      </c>
-      <c r="S9" s="1">
-        <v>297</v>
-      </c>
-      <c r="T9" s="1">
-        <v>300</v>
-      </c>
-      <c r="U9" s="1">
-        <v>300</v>
-      </c>
-      <c r="V9" s="1">
-        <v>300</v>
-      </c>
-      <c r="W9" s="1">
-        <v>300</v>
-      </c>
-      <c r="X9" s="1">
-        <v>300</v>
-      </c>
-      <c r="Y9" s="1">
-        <v>300</v>
-      </c>
-      <c r="Z9" s="1">
-        <v>172</v>
-      </c>
-      <c r="AA9" s="1">
-        <v>300</v>
-      </c>
-      <c r="AB9" s="1">
-        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
@@ -27681,6 +27681,92 @@
       </c>
       <c r="AB311" s="8">
         <v>1.2</v>
+      </c>
+    </row>
+    <row r="312" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A312" s="9">
+        <v>45261</v>
+      </c>
+      <c r="B312" s="8">
+        <v>136.4</v>
+      </c>
+      <c r="C312" s="8">
+        <v>136.1</v>
+      </c>
+      <c r="D312" s="8">
+        <v>137.69999999999999</v>
+      </c>
+      <c r="E312" s="8">
+        <v>137.1</v>
+      </c>
+      <c r="F312" s="8">
+        <v>134</v>
+      </c>
+      <c r="G312" s="8">
+        <v>136.80000000000001</v>
+      </c>
+      <c r="H312" s="8">
+        <v>131.5</v>
+      </c>
+      <c r="I312" s="8">
+        <v>134.30000000000001</v>
+      </c>
+      <c r="J312" s="8">
+        <v>136.1</v>
+      </c>
+      <c r="K312" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="L312" s="8">
+        <v>3.8</v>
+      </c>
+      <c r="M312" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="N312" s="8">
+        <v>4.8</v>
+      </c>
+      <c r="O312" s="8">
+        <v>3.6</v>
+      </c>
+      <c r="P312" s="8">
+        <v>3.3</v>
+      </c>
+      <c r="Q312" s="8">
+        <v>3.9</v>
+      </c>
+      <c r="R312" s="8">
+        <v>3.7</v>
+      </c>
+      <c r="S312" s="8">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="T312" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="U312" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="V312" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="W312" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="X312" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="Y312" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="Z312" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="AA312" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="AB312" s="8">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to 2023 data. Update.R script modified.
</commit_message>
<xml_diff>
--- a/data/cpi.xlsx
+++ b/data/cpi.xlsx
@@ -17,89 +17,89 @@
     <sheet name="Enquiries" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="A2325806K">Data1!$B$1:$B$10,Data1!$B$11:$B$312</definedName>
-    <definedName name="A2325806K_Data">Data1!$B$11:$B$312</definedName>
-    <definedName name="A2325806K_Latest">Data1!$B$312</definedName>
-    <definedName name="A2325807L">Data1!$K$1:$K$10,Data1!$K$15:$K$312</definedName>
-    <definedName name="A2325807L_Data">Data1!$K$15:$K$312</definedName>
-    <definedName name="A2325807L_Latest">Data1!$K$312</definedName>
-    <definedName name="A2325810A">Data1!$T$1:$T$10,Data1!$T$12:$T$312</definedName>
-    <definedName name="A2325810A_Data">Data1!$T$12:$T$312</definedName>
-    <definedName name="A2325810A_Latest">Data1!$T$312</definedName>
-    <definedName name="A2325811C">Data1!$C$1:$C$10,Data1!$C$11:$C$312</definedName>
-    <definedName name="A2325811C_Data">Data1!$C$11:$C$312</definedName>
-    <definedName name="A2325811C_Latest">Data1!$C$312</definedName>
-    <definedName name="A2325812F">Data1!$L$1:$L$10,Data1!$L$15:$L$312</definedName>
-    <definedName name="A2325812F_Data">Data1!$L$15:$L$312</definedName>
-    <definedName name="A2325812F_Latest">Data1!$L$312</definedName>
-    <definedName name="A2325815L">Data1!$U$1:$U$10,Data1!$U$12:$U$312</definedName>
-    <definedName name="A2325815L_Data">Data1!$U$12:$U$312</definedName>
-    <definedName name="A2325815L_Latest">Data1!$U$312</definedName>
-    <definedName name="A2325816R">Data1!$D$1:$D$10,Data1!$D$11:$D$312</definedName>
-    <definedName name="A2325816R_Data">Data1!$D$11:$D$312</definedName>
-    <definedName name="A2325816R_Latest">Data1!$D$312</definedName>
-    <definedName name="A2325817T">Data1!$M$1:$M$10,Data1!$M$15:$M$312</definedName>
-    <definedName name="A2325817T_Data">Data1!$M$15:$M$312</definedName>
-    <definedName name="A2325817T_Latest">Data1!$M$312</definedName>
-    <definedName name="A2325820F">Data1!$V$1:$V$10,Data1!$V$12:$V$312</definedName>
-    <definedName name="A2325820F_Data">Data1!$V$12:$V$312</definedName>
-    <definedName name="A2325820F_Latest">Data1!$V$312</definedName>
-    <definedName name="A2325821J">Data1!$E$1:$E$10,Data1!$E$11:$E$312</definedName>
-    <definedName name="A2325821J_Data">Data1!$E$11:$E$312</definedName>
-    <definedName name="A2325821J_Latest">Data1!$E$312</definedName>
-    <definedName name="A2325822K">Data1!$N$1:$N$10,Data1!$N$15:$N$312</definedName>
-    <definedName name="A2325822K_Data">Data1!$N$15:$N$312</definedName>
-    <definedName name="A2325822K_Latest">Data1!$N$312</definedName>
-    <definedName name="A2325825T">Data1!$W$1:$W$10,Data1!$W$12:$W$312</definedName>
-    <definedName name="A2325825T_Data">Data1!$W$12:$W$312</definedName>
-    <definedName name="A2325825T_Latest">Data1!$W$312</definedName>
-    <definedName name="A2325826V">Data1!$F$1:$F$10,Data1!$F$11:$F$312</definedName>
-    <definedName name="A2325826V_Data">Data1!$F$11:$F$312</definedName>
-    <definedName name="A2325826V_Latest">Data1!$F$312</definedName>
-    <definedName name="A2325827W">Data1!$O$1:$O$10,Data1!$O$15:$O$312</definedName>
-    <definedName name="A2325827W_Data">Data1!$O$15:$O$312</definedName>
-    <definedName name="A2325827W_Latest">Data1!$O$312</definedName>
-    <definedName name="A2325830K">Data1!$X$1:$X$10,Data1!$X$12:$X$312</definedName>
-    <definedName name="A2325830K_Data">Data1!$X$12:$X$312</definedName>
-    <definedName name="A2325830K_Latest">Data1!$X$312</definedName>
-    <definedName name="A2325831L">Data1!$G$1:$G$10,Data1!$G$11:$G$312</definedName>
-    <definedName name="A2325831L_Data">Data1!$G$11:$G$312</definedName>
-    <definedName name="A2325831L_Latest">Data1!$G$312</definedName>
-    <definedName name="A2325832R">Data1!$P$1:$P$10,Data1!$P$15:$P$312</definedName>
-    <definedName name="A2325832R_Data">Data1!$P$15:$P$312</definedName>
-    <definedName name="A2325832R_Latest">Data1!$P$312</definedName>
-    <definedName name="A2325835W">Data1!$Y$1:$Y$10,Data1!$Y$12:$Y$312</definedName>
-    <definedName name="A2325835W_Data">Data1!$Y$12:$Y$312</definedName>
-    <definedName name="A2325835W_Latest">Data1!$Y$312</definedName>
-    <definedName name="A2325836X">Data1!$H$1:$H$10,Data1!$H$139:$H$312</definedName>
-    <definedName name="A2325836X_Data">Data1!$H$139:$H$312</definedName>
-    <definedName name="A2325836X_Latest">Data1!$H$312</definedName>
-    <definedName name="A2325837A">Data1!$Q$1:$Q$10,Data1!$Q$143:$Q$312</definedName>
-    <definedName name="A2325837A_Data">Data1!$Q$143:$Q$312</definedName>
-    <definedName name="A2325837A_Latest">Data1!$Q$312</definedName>
-    <definedName name="A2325840R">Data1!$Z$1:$Z$10,Data1!$Z$140:$Z$312</definedName>
-    <definedName name="A2325840R_Data">Data1!$Z$140:$Z$312</definedName>
-    <definedName name="A2325840R_Latest">Data1!$Z$312</definedName>
-    <definedName name="A2325841T">Data1!$I$1:$I$10,Data1!$I$11:$I$312</definedName>
-    <definedName name="A2325841T_Data">Data1!$I$11:$I$312</definedName>
-    <definedName name="A2325841T_Latest">Data1!$I$312</definedName>
-    <definedName name="A2325842V">Data1!$R$1:$R$10,Data1!$R$15:$R$312</definedName>
-    <definedName name="A2325842V_Data">Data1!$R$15:$R$312</definedName>
-    <definedName name="A2325842V_Latest">Data1!$R$312</definedName>
-    <definedName name="A2325845A">Data1!$AA$1:$AA$10,Data1!$AA$12:$AA$312</definedName>
-    <definedName name="A2325845A_Data">Data1!$AA$12:$AA$312</definedName>
-    <definedName name="A2325845A_Latest">Data1!$AA$312</definedName>
-    <definedName name="A2325846C">Data1!$J$1:$J$10,Data1!$J$11:$J$312</definedName>
-    <definedName name="A2325846C_Data">Data1!$J$11:$J$312</definedName>
-    <definedName name="A2325846C_Latest">Data1!$J$312</definedName>
-    <definedName name="A2325847F">Data1!$S$1:$S$10,Data1!$S$15:$S$312</definedName>
-    <definedName name="A2325847F_Data">Data1!$S$15:$S$312</definedName>
-    <definedName name="A2325847F_Latest">Data1!$S$312</definedName>
-    <definedName name="A2325850V">Data1!$AB$1:$AB$10,Data1!$AB$12:$AB$312</definedName>
-    <definedName name="A2325850V_Data">Data1!$AB$12:$AB$312</definedName>
-    <definedName name="A2325850V_Latest">Data1!$AB$312</definedName>
-    <definedName name="Date_Range">Data1!$A$2:$A$10,Data1!$A$11:$A$312</definedName>
-    <definedName name="Date_Range_Data">Data1!$A$11:$A$312</definedName>
+    <definedName name="A2325806K">Data1!$B$1:$B$10,Data1!$B$11:$B$315</definedName>
+    <definedName name="A2325806K_Data">Data1!$B$11:$B$315</definedName>
+    <definedName name="A2325806K_Latest">Data1!$B$315</definedName>
+    <definedName name="A2325807L">Data1!$K$1:$K$10,Data1!$K$15:$K$315</definedName>
+    <definedName name="A2325807L_Data">Data1!$K$15:$K$315</definedName>
+    <definedName name="A2325807L_Latest">Data1!$K$315</definedName>
+    <definedName name="A2325810A">Data1!$T$1:$T$10,Data1!$T$12:$T$315</definedName>
+    <definedName name="A2325810A_Data">Data1!$T$12:$T$315</definedName>
+    <definedName name="A2325810A_Latest">Data1!$T$315</definedName>
+    <definedName name="A2325811C">Data1!$C$1:$C$10,Data1!$C$11:$C$315</definedName>
+    <definedName name="A2325811C_Data">Data1!$C$11:$C$315</definedName>
+    <definedName name="A2325811C_Latest">Data1!$C$315</definedName>
+    <definedName name="A2325812F">Data1!$L$1:$L$10,Data1!$L$15:$L$315</definedName>
+    <definedName name="A2325812F_Data">Data1!$L$15:$L$315</definedName>
+    <definedName name="A2325812F_Latest">Data1!$L$315</definedName>
+    <definedName name="A2325815L">Data1!$U$1:$U$10,Data1!$U$12:$U$315</definedName>
+    <definedName name="A2325815L_Data">Data1!$U$12:$U$315</definedName>
+    <definedName name="A2325815L_Latest">Data1!$U$315</definedName>
+    <definedName name="A2325816R">Data1!$D$1:$D$10,Data1!$D$11:$D$315</definedName>
+    <definedName name="A2325816R_Data">Data1!$D$11:$D$315</definedName>
+    <definedName name="A2325816R_Latest">Data1!$D$315</definedName>
+    <definedName name="A2325817T">Data1!$M$1:$M$10,Data1!$M$15:$M$315</definedName>
+    <definedName name="A2325817T_Data">Data1!$M$15:$M$315</definedName>
+    <definedName name="A2325817T_Latest">Data1!$M$315</definedName>
+    <definedName name="A2325820F">Data1!$V$1:$V$10,Data1!$V$12:$V$315</definedName>
+    <definedName name="A2325820F_Data">Data1!$V$12:$V$315</definedName>
+    <definedName name="A2325820F_Latest">Data1!$V$315</definedName>
+    <definedName name="A2325821J">Data1!$E$1:$E$10,Data1!$E$11:$E$315</definedName>
+    <definedName name="A2325821J_Data">Data1!$E$11:$E$315</definedName>
+    <definedName name="A2325821J_Latest">Data1!$E$315</definedName>
+    <definedName name="A2325822K">Data1!$N$1:$N$10,Data1!$N$15:$N$315</definedName>
+    <definedName name="A2325822K_Data">Data1!$N$15:$N$315</definedName>
+    <definedName name="A2325822K_Latest">Data1!$N$315</definedName>
+    <definedName name="A2325825T">Data1!$W$1:$W$10,Data1!$W$12:$W$315</definedName>
+    <definedName name="A2325825T_Data">Data1!$W$12:$W$315</definedName>
+    <definedName name="A2325825T_Latest">Data1!$W$315</definedName>
+    <definedName name="A2325826V">Data1!$F$1:$F$10,Data1!$F$11:$F$315</definedName>
+    <definedName name="A2325826V_Data">Data1!$F$11:$F$315</definedName>
+    <definedName name="A2325826V_Latest">Data1!$F$315</definedName>
+    <definedName name="A2325827W">Data1!$O$1:$O$10,Data1!$O$15:$O$315</definedName>
+    <definedName name="A2325827W_Data">Data1!$O$15:$O$315</definedName>
+    <definedName name="A2325827W_Latest">Data1!$O$315</definedName>
+    <definedName name="A2325830K">Data1!$X$1:$X$10,Data1!$X$12:$X$315</definedName>
+    <definedName name="A2325830K_Data">Data1!$X$12:$X$315</definedName>
+    <definedName name="A2325830K_Latest">Data1!$X$315</definedName>
+    <definedName name="A2325831L">Data1!$G$1:$G$10,Data1!$G$11:$G$315</definedName>
+    <definedName name="A2325831L_Data">Data1!$G$11:$G$315</definedName>
+    <definedName name="A2325831L_Latest">Data1!$G$315</definedName>
+    <definedName name="A2325832R">Data1!$P$1:$P$10,Data1!$P$15:$P$315</definedName>
+    <definedName name="A2325832R_Data">Data1!$P$15:$P$315</definedName>
+    <definedName name="A2325832R_Latest">Data1!$P$315</definedName>
+    <definedName name="A2325835W">Data1!$Y$1:$Y$10,Data1!$Y$12:$Y$315</definedName>
+    <definedName name="A2325835W_Data">Data1!$Y$12:$Y$315</definedName>
+    <definedName name="A2325835W_Latest">Data1!$Y$315</definedName>
+    <definedName name="A2325836X">Data1!$H$1:$H$10,Data1!$H$139:$H$315</definedName>
+    <definedName name="A2325836X_Data">Data1!$H$139:$H$315</definedName>
+    <definedName name="A2325836X_Latest">Data1!$H$315</definedName>
+    <definedName name="A2325837A">Data1!$Q$1:$Q$10,Data1!$Q$143:$Q$315</definedName>
+    <definedName name="A2325837A_Data">Data1!$Q$143:$Q$315</definedName>
+    <definedName name="A2325837A_Latest">Data1!$Q$315</definedName>
+    <definedName name="A2325840R">Data1!$Z$1:$Z$10,Data1!$Z$140:$Z$315</definedName>
+    <definedName name="A2325840R_Data">Data1!$Z$140:$Z$315</definedName>
+    <definedName name="A2325840R_Latest">Data1!$Z$315</definedName>
+    <definedName name="A2325841T">Data1!$I$1:$I$10,Data1!$I$11:$I$315</definedName>
+    <definedName name="A2325841T_Data">Data1!$I$11:$I$315</definedName>
+    <definedName name="A2325841T_Latest">Data1!$I$315</definedName>
+    <definedName name="A2325842V">Data1!$R$1:$R$10,Data1!$R$15:$R$315</definedName>
+    <definedName name="A2325842V_Data">Data1!$R$15:$R$315</definedName>
+    <definedName name="A2325842V_Latest">Data1!$R$315</definedName>
+    <definedName name="A2325845A">Data1!$AA$1:$AA$10,Data1!$AA$12:$AA$315</definedName>
+    <definedName name="A2325845A_Data">Data1!$AA$12:$AA$315</definedName>
+    <definedName name="A2325845A_Latest">Data1!$AA$315</definedName>
+    <definedName name="A2325846C">Data1!$J$1:$J$10,Data1!$J$11:$J$315</definedName>
+    <definedName name="A2325846C_Data">Data1!$J$11:$J$315</definedName>
+    <definedName name="A2325846C_Latest">Data1!$J$315</definedName>
+    <definedName name="A2325847F">Data1!$S$1:$S$10,Data1!$S$15:$S$315</definedName>
+    <definedName name="A2325847F_Data">Data1!$S$15:$S$315</definedName>
+    <definedName name="A2325847F_Latest">Data1!$S$315</definedName>
+    <definedName name="A2325850V">Data1!$AB$1:$AB$10,Data1!$AB$12:$AB$315</definedName>
+    <definedName name="A2325850V_Data">Data1!$AB$12:$AB$315</definedName>
+    <definedName name="A2325850V_Latest">Data1!$AB$315</definedName>
+    <definedName name="Date_Range">Data1!$A$2:$A$10,Data1!$A$11:$A$315</definedName>
+    <definedName name="Date_Range_Data">Data1!$A$11:$A$315</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1316,10 +1316,10 @@
         <v>17777</v>
       </c>
       <c r="G12" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H12" s="10">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>36</v>
@@ -1348,10 +1348,10 @@
         <v>17777</v>
       </c>
       <c r="G13" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H13" s="10">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>36</v>
@@ -1380,10 +1380,10 @@
         <v>17777</v>
       </c>
       <c r="G14" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H14" s="10">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>36</v>
@@ -1412,10 +1412,10 @@
         <v>17777</v>
       </c>
       <c r="G15" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H15" s="10">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>36</v>
@@ -1444,10 +1444,10 @@
         <v>17777</v>
       </c>
       <c r="G16" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H16" s="10">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>36</v>
@@ -1476,10 +1476,10 @@
         <v>17777</v>
       </c>
       <c r="G17" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H17" s="10">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>36</v>
@@ -1508,10 +1508,10 @@
         <v>29465</v>
       </c>
       <c r="G18" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H18" s="10">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>36</v>
@@ -1540,10 +1540,10 @@
         <v>17777</v>
       </c>
       <c r="G19" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H19" s="10">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>36</v>
@@ -1572,10 +1572,10 @@
         <v>17777</v>
       </c>
       <c r="G20" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H20" s="10">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>36</v>
@@ -1604,10 +1604,10 @@
         <v>18142</v>
       </c>
       <c r="G21" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H21" s="10">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>49</v>
@@ -1636,10 +1636,10 @@
         <v>18142</v>
       </c>
       <c r="G22" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H22" s="10">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>49</v>
@@ -1668,10 +1668,10 @@
         <v>18142</v>
       </c>
       <c r="G23" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H23" s="10">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>49</v>
@@ -1700,10 +1700,10 @@
         <v>18142</v>
       </c>
       <c r="G24" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H24" s="10">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>49</v>
@@ -1732,10 +1732,10 @@
         <v>18142</v>
       </c>
       <c r="G25" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H25" s="10">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>49</v>
@@ -1764,10 +1764,10 @@
         <v>18142</v>
       </c>
       <c r="G26" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H26" s="10">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>49</v>
@@ -1796,10 +1796,10 @@
         <v>29830</v>
       </c>
       <c r="G27" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H27" s="10">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>49</v>
@@ -1828,10 +1828,10 @@
         <v>18142</v>
       </c>
       <c r="G28" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H28" s="10">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>49</v>
@@ -1860,10 +1860,10 @@
         <v>18142</v>
       </c>
       <c r="G29" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H29" s="10">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>49</v>
@@ -1892,10 +1892,10 @@
         <v>17868</v>
       </c>
       <c r="G30" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H30" s="10">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>49</v>
@@ -1924,10 +1924,10 @@
         <v>17868</v>
       </c>
       <c r="G31" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H31" s="10">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>49</v>
@@ -1956,10 +1956,10 @@
         <v>17868</v>
       </c>
       <c r="G32" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H32" s="10">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>49</v>
@@ -1988,10 +1988,10 @@
         <v>17868</v>
       </c>
       <c r="G33" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H33" s="10">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>49</v>
@@ -2020,10 +2020,10 @@
         <v>17868</v>
       </c>
       <c r="G34" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H34" s="10">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>49</v>
@@ -2052,10 +2052,10 @@
         <v>17868</v>
       </c>
       <c r="G35" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H35" s="10">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>49</v>
@@ -2084,10 +2084,10 @@
         <v>29556</v>
       </c>
       <c r="G36" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H36" s="10">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="I36" s="10" t="s">
         <v>49</v>
@@ -2116,10 +2116,10 @@
         <v>17868</v>
       </c>
       <c r="G37" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H37" s="10">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="I37" s="10" t="s">
         <v>49</v>
@@ -2148,10 +2148,10 @@
         <v>17868</v>
       </c>
       <c r="G38" s="9">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H38" s="10">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>49</v>
@@ -2213,7 +2213,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB312"/>
+  <dimension ref="A1:AB315"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
@@ -2831,85 +2831,85 @@
         <v>33</v>
       </c>
       <c r="B8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="C8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="D8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="E8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="F8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="G8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="H8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="I8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="J8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="K8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="L8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="M8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="N8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="O8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="P8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="Q8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="R8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="S8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="T8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="U8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="V8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="W8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="X8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="Y8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="Z8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="AA8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
       <c r="AB8" s="6">
-        <v>45261</v>
+        <v>45536</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
@@ -2917,85 +2917,85 @@
         <v>34</v>
       </c>
       <c r="B9" s="1">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="C9" s="1">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D9" s="1">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="E9" s="1">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="F9" s="1">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="G9" s="1">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="H9" s="1">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="I9" s="1">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="J9" s="1">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="K9" s="1">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="L9" s="1">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="M9" s="1">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="N9" s="1">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="O9" s="1">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="P9" s="1">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="Q9" s="1">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="R9" s="1">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="S9" s="1">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="T9" s="1">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="U9" s="1">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="V9" s="1">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="W9" s="1">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="X9" s="1">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="Y9" s="1">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="Z9" s="1">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="AA9" s="1">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="AB9" s="1">
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
@@ -27767,6 +27767,264 @@
       </c>
       <c r="AB312" s="8">
         <v>0.6</v>
+      </c>
+    </row>
+    <row r="313" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A313" s="9">
+        <v>45352</v>
+      </c>
+      <c r="B313" s="8">
+        <v>137.69999999999999</v>
+      </c>
+      <c r="C313" s="8">
+        <v>137.5</v>
+      </c>
+      <c r="D313" s="8">
+        <v>139.19999999999999</v>
+      </c>
+      <c r="E313" s="8">
+        <v>138.1</v>
+      </c>
+      <c r="F313" s="8">
+        <v>134.80000000000001</v>
+      </c>
+      <c r="G313" s="8">
+        <v>138.1</v>
+      </c>
+      <c r="H313" s="8">
+        <v>132.4</v>
+      </c>
+      <c r="I313" s="8">
+        <v>135.6</v>
+      </c>
+      <c r="J313" s="8">
+        <v>137.4</v>
+      </c>
+      <c r="K313" s="8">
+        <v>3.8</v>
+      </c>
+      <c r="L313" s="8">
+        <v>3.6</v>
+      </c>
+      <c r="M313" s="8">
+        <v>3.4</v>
+      </c>
+      <c r="N313" s="8">
+        <v>4.3</v>
+      </c>
+      <c r="O313" s="8">
+        <v>3.4</v>
+      </c>
+      <c r="P313" s="8">
+        <v>3.1</v>
+      </c>
+      <c r="Q313" s="8">
+        <v>3.3</v>
+      </c>
+      <c r="R313" s="8">
+        <v>3.3</v>
+      </c>
+      <c r="S313" s="8">
+        <v>3.6</v>
+      </c>
+      <c r="T313" s="8">
+        <v>1</v>
+      </c>
+      <c r="U313" s="8">
+        <v>1</v>
+      </c>
+      <c r="V313" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W313" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="X313" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="Y313" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z313" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="AA313" s="8">
+        <v>1</v>
+      </c>
+      <c r="AB313" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A314" s="9">
+        <v>45444</v>
+      </c>
+      <c r="B314" s="8">
+        <v>139.1</v>
+      </c>
+      <c r="C314" s="8">
+        <v>138.4</v>
+      </c>
+      <c r="D314" s="8">
+        <v>140.6</v>
+      </c>
+      <c r="E314" s="8">
+        <v>139.9</v>
+      </c>
+      <c r="F314" s="8">
+        <v>137.6</v>
+      </c>
+      <c r="G314" s="8">
+        <v>138.30000000000001</v>
+      </c>
+      <c r="H314" s="8">
+        <v>133.6</v>
+      </c>
+      <c r="I314" s="8">
+        <v>136.80000000000001</v>
+      </c>
+      <c r="J314" s="8">
+        <v>138.80000000000001</v>
+      </c>
+      <c r="K314" s="8">
+        <v>3.8</v>
+      </c>
+      <c r="L314" s="8">
+        <v>3.7</v>
+      </c>
+      <c r="M314" s="8">
+        <v>3.4</v>
+      </c>
+      <c r="N314" s="8">
+        <v>4.5</v>
+      </c>
+      <c r="O314" s="8">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="P314" s="8">
+        <v>2.7</v>
+      </c>
+      <c r="Q314" s="8">
+        <v>3</v>
+      </c>
+      <c r="R314" s="8">
+        <v>3.1</v>
+      </c>
+      <c r="S314" s="8">
+        <v>3.8</v>
+      </c>
+      <c r="T314" s="8">
+        <v>1</v>
+      </c>
+      <c r="U314" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="V314" s="8">
+        <v>1</v>
+      </c>
+      <c r="W314" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="X314" s="8">
+        <v>2.1</v>
+      </c>
+      <c r="Y314" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="Z314" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="AA314" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="AB314" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A315" s="9">
+        <v>45536</v>
+      </c>
+      <c r="B315" s="8">
+        <v>139.80000000000001</v>
+      </c>
+      <c r="C315" s="8">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="D315" s="8">
+        <v>139.4</v>
+      </c>
+      <c r="E315" s="8">
+        <v>140.6</v>
+      </c>
+      <c r="F315" s="8">
+        <v>137</v>
+      </c>
+      <c r="G315" s="8">
+        <v>136.80000000000001</v>
+      </c>
+      <c r="H315" s="8">
+        <v>133.80000000000001</v>
+      </c>
+      <c r="I315" s="8">
+        <v>137.19999999999999</v>
+      </c>
+      <c r="J315" s="8">
+        <v>139.1</v>
+      </c>
+      <c r="K315" s="8">
+        <v>2.9</v>
+      </c>
+      <c r="L315" s="8">
+        <v>3</v>
+      </c>
+      <c r="M315" s="8">
+        <v>1.8</v>
+      </c>
+      <c r="N315" s="8">
+        <v>3.2</v>
+      </c>
+      <c r="O315" s="8">
+        <v>3.8</v>
+      </c>
+      <c r="P315" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="Q315" s="8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R315" s="8">
+        <v>2.6</v>
+      </c>
+      <c r="S315" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="T315" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="U315" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="V315" s="8">
+        <v>-0.9</v>
+      </c>
+      <c r="W315" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="X315" s="8">
+        <v>-0.4</v>
+      </c>
+      <c r="Y315" s="8">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="Z315" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="AA315" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="AB315" s="8">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated updater function. Ran updater to now include 2024 data.
</commit_message>
<xml_diff>
--- a/data/cpi.xlsx
+++ b/data/cpi.xlsx
@@ -17,89 +17,89 @@
     <sheet name="Enquiries" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="A2325806K">Data1!$B$1:$B$10,Data1!$B$11:$B$315</definedName>
-    <definedName name="A2325806K_Data">Data1!$B$11:$B$315</definedName>
-    <definedName name="A2325806K_Latest">Data1!$B$315</definedName>
-    <definedName name="A2325807L">Data1!$K$1:$K$10,Data1!$K$15:$K$315</definedName>
-    <definedName name="A2325807L_Data">Data1!$K$15:$K$315</definedName>
-    <definedName name="A2325807L_Latest">Data1!$K$315</definedName>
-    <definedName name="A2325810A">Data1!$T$1:$T$10,Data1!$T$12:$T$315</definedName>
-    <definedName name="A2325810A_Data">Data1!$T$12:$T$315</definedName>
-    <definedName name="A2325810A_Latest">Data1!$T$315</definedName>
-    <definedName name="A2325811C">Data1!$C$1:$C$10,Data1!$C$11:$C$315</definedName>
-    <definedName name="A2325811C_Data">Data1!$C$11:$C$315</definedName>
-    <definedName name="A2325811C_Latest">Data1!$C$315</definedName>
-    <definedName name="A2325812F">Data1!$L$1:$L$10,Data1!$L$15:$L$315</definedName>
-    <definedName name="A2325812F_Data">Data1!$L$15:$L$315</definedName>
-    <definedName name="A2325812F_Latest">Data1!$L$315</definedName>
-    <definedName name="A2325815L">Data1!$U$1:$U$10,Data1!$U$12:$U$315</definedName>
-    <definedName name="A2325815L_Data">Data1!$U$12:$U$315</definedName>
-    <definedName name="A2325815L_Latest">Data1!$U$315</definedName>
-    <definedName name="A2325816R">Data1!$D$1:$D$10,Data1!$D$11:$D$315</definedName>
-    <definedName name="A2325816R_Data">Data1!$D$11:$D$315</definedName>
-    <definedName name="A2325816R_Latest">Data1!$D$315</definedName>
-    <definedName name="A2325817T">Data1!$M$1:$M$10,Data1!$M$15:$M$315</definedName>
-    <definedName name="A2325817T_Data">Data1!$M$15:$M$315</definedName>
-    <definedName name="A2325817T_Latest">Data1!$M$315</definedName>
-    <definedName name="A2325820F">Data1!$V$1:$V$10,Data1!$V$12:$V$315</definedName>
-    <definedName name="A2325820F_Data">Data1!$V$12:$V$315</definedName>
-    <definedName name="A2325820F_Latest">Data1!$V$315</definedName>
-    <definedName name="A2325821J">Data1!$E$1:$E$10,Data1!$E$11:$E$315</definedName>
-    <definedName name="A2325821J_Data">Data1!$E$11:$E$315</definedName>
-    <definedName name="A2325821J_Latest">Data1!$E$315</definedName>
-    <definedName name="A2325822K">Data1!$N$1:$N$10,Data1!$N$15:$N$315</definedName>
-    <definedName name="A2325822K_Data">Data1!$N$15:$N$315</definedName>
-    <definedName name="A2325822K_Latest">Data1!$N$315</definedName>
-    <definedName name="A2325825T">Data1!$W$1:$W$10,Data1!$W$12:$W$315</definedName>
-    <definedName name="A2325825T_Data">Data1!$W$12:$W$315</definedName>
-    <definedName name="A2325825T_Latest">Data1!$W$315</definedName>
-    <definedName name="A2325826V">Data1!$F$1:$F$10,Data1!$F$11:$F$315</definedName>
-    <definedName name="A2325826V_Data">Data1!$F$11:$F$315</definedName>
-    <definedName name="A2325826V_Latest">Data1!$F$315</definedName>
-    <definedName name="A2325827W">Data1!$O$1:$O$10,Data1!$O$15:$O$315</definedName>
-    <definedName name="A2325827W_Data">Data1!$O$15:$O$315</definedName>
-    <definedName name="A2325827W_Latest">Data1!$O$315</definedName>
-    <definedName name="A2325830K">Data1!$X$1:$X$10,Data1!$X$12:$X$315</definedName>
-    <definedName name="A2325830K_Data">Data1!$X$12:$X$315</definedName>
-    <definedName name="A2325830K_Latest">Data1!$X$315</definedName>
-    <definedName name="A2325831L">Data1!$G$1:$G$10,Data1!$G$11:$G$315</definedName>
-    <definedName name="A2325831L_Data">Data1!$G$11:$G$315</definedName>
-    <definedName name="A2325831L_Latest">Data1!$G$315</definedName>
-    <definedName name="A2325832R">Data1!$P$1:$P$10,Data1!$P$15:$P$315</definedName>
-    <definedName name="A2325832R_Data">Data1!$P$15:$P$315</definedName>
-    <definedName name="A2325832R_Latest">Data1!$P$315</definedName>
-    <definedName name="A2325835W">Data1!$Y$1:$Y$10,Data1!$Y$12:$Y$315</definedName>
-    <definedName name="A2325835W_Data">Data1!$Y$12:$Y$315</definedName>
-    <definedName name="A2325835W_Latest">Data1!$Y$315</definedName>
-    <definedName name="A2325836X">Data1!$H$1:$H$10,Data1!$H$139:$H$315</definedName>
-    <definedName name="A2325836X_Data">Data1!$H$139:$H$315</definedName>
-    <definedName name="A2325836X_Latest">Data1!$H$315</definedName>
-    <definedName name="A2325837A">Data1!$Q$1:$Q$10,Data1!$Q$143:$Q$315</definedName>
-    <definedName name="A2325837A_Data">Data1!$Q$143:$Q$315</definedName>
-    <definedName name="A2325837A_Latest">Data1!$Q$315</definedName>
-    <definedName name="A2325840R">Data1!$Z$1:$Z$10,Data1!$Z$140:$Z$315</definedName>
-    <definedName name="A2325840R_Data">Data1!$Z$140:$Z$315</definedName>
-    <definedName name="A2325840R_Latest">Data1!$Z$315</definedName>
-    <definedName name="A2325841T">Data1!$I$1:$I$10,Data1!$I$11:$I$315</definedName>
-    <definedName name="A2325841T_Data">Data1!$I$11:$I$315</definedName>
-    <definedName name="A2325841T_Latest">Data1!$I$315</definedName>
-    <definedName name="A2325842V">Data1!$R$1:$R$10,Data1!$R$15:$R$315</definedName>
-    <definedName name="A2325842V_Data">Data1!$R$15:$R$315</definedName>
-    <definedName name="A2325842V_Latest">Data1!$R$315</definedName>
-    <definedName name="A2325845A">Data1!$AA$1:$AA$10,Data1!$AA$12:$AA$315</definedName>
-    <definedName name="A2325845A_Data">Data1!$AA$12:$AA$315</definedName>
-    <definedName name="A2325845A_Latest">Data1!$AA$315</definedName>
-    <definedName name="A2325846C">Data1!$J$1:$J$10,Data1!$J$11:$J$315</definedName>
-    <definedName name="A2325846C_Data">Data1!$J$11:$J$315</definedName>
-    <definedName name="A2325846C_Latest">Data1!$J$315</definedName>
-    <definedName name="A2325847F">Data1!$S$1:$S$10,Data1!$S$15:$S$315</definedName>
-    <definedName name="A2325847F_Data">Data1!$S$15:$S$315</definedName>
-    <definedName name="A2325847F_Latest">Data1!$S$315</definedName>
-    <definedName name="A2325850V">Data1!$AB$1:$AB$10,Data1!$AB$12:$AB$315</definedName>
-    <definedName name="A2325850V_Data">Data1!$AB$12:$AB$315</definedName>
-    <definedName name="A2325850V_Latest">Data1!$AB$315</definedName>
-    <definedName name="Date_Range">Data1!$A$2:$A$10,Data1!$A$11:$A$315</definedName>
-    <definedName name="Date_Range_Data">Data1!$A$11:$A$315</definedName>
+    <definedName name="A2325806K">Data1!$B$1:$B$10,Data1!$B$11:$B$317</definedName>
+    <definedName name="A2325806K_Data">Data1!$B$11:$B$317</definedName>
+    <definedName name="A2325806K_Latest">Data1!$B$317</definedName>
+    <definedName name="A2325807L">Data1!$K$1:$K$10,Data1!$K$15:$K$317</definedName>
+    <definedName name="A2325807L_Data">Data1!$K$15:$K$317</definedName>
+    <definedName name="A2325807L_Latest">Data1!$K$317</definedName>
+    <definedName name="A2325810A">Data1!$T$1:$T$10,Data1!$T$12:$T$317</definedName>
+    <definedName name="A2325810A_Data">Data1!$T$12:$T$317</definedName>
+    <definedName name="A2325810A_Latest">Data1!$T$317</definedName>
+    <definedName name="A2325811C">Data1!$C$1:$C$10,Data1!$C$11:$C$317</definedName>
+    <definedName name="A2325811C_Data">Data1!$C$11:$C$317</definedName>
+    <definedName name="A2325811C_Latest">Data1!$C$317</definedName>
+    <definedName name="A2325812F">Data1!$L$1:$L$10,Data1!$L$15:$L$317</definedName>
+    <definedName name="A2325812F_Data">Data1!$L$15:$L$317</definedName>
+    <definedName name="A2325812F_Latest">Data1!$L$317</definedName>
+    <definedName name="A2325815L">Data1!$U$1:$U$10,Data1!$U$12:$U$317</definedName>
+    <definedName name="A2325815L_Data">Data1!$U$12:$U$317</definedName>
+    <definedName name="A2325815L_Latest">Data1!$U$317</definedName>
+    <definedName name="A2325816R">Data1!$D$1:$D$10,Data1!$D$11:$D$317</definedName>
+    <definedName name="A2325816R_Data">Data1!$D$11:$D$317</definedName>
+    <definedName name="A2325816R_Latest">Data1!$D$317</definedName>
+    <definedName name="A2325817T">Data1!$M$1:$M$10,Data1!$M$15:$M$317</definedName>
+    <definedName name="A2325817T_Data">Data1!$M$15:$M$317</definedName>
+    <definedName name="A2325817T_Latest">Data1!$M$317</definedName>
+    <definedName name="A2325820F">Data1!$V$1:$V$10,Data1!$V$12:$V$317</definedName>
+    <definedName name="A2325820F_Data">Data1!$V$12:$V$317</definedName>
+    <definedName name="A2325820F_Latest">Data1!$V$317</definedName>
+    <definedName name="A2325821J">Data1!$E$1:$E$10,Data1!$E$11:$E$317</definedName>
+    <definedName name="A2325821J_Data">Data1!$E$11:$E$317</definedName>
+    <definedName name="A2325821J_Latest">Data1!$E$317</definedName>
+    <definedName name="A2325822K">Data1!$N$1:$N$10,Data1!$N$15:$N$317</definedName>
+    <definedName name="A2325822K_Data">Data1!$N$15:$N$317</definedName>
+    <definedName name="A2325822K_Latest">Data1!$N$317</definedName>
+    <definedName name="A2325825T">Data1!$W$1:$W$10,Data1!$W$12:$W$317</definedName>
+    <definedName name="A2325825T_Data">Data1!$W$12:$W$317</definedName>
+    <definedName name="A2325825T_Latest">Data1!$W$317</definedName>
+    <definedName name="A2325826V">Data1!$F$1:$F$10,Data1!$F$11:$F$317</definedName>
+    <definedName name="A2325826V_Data">Data1!$F$11:$F$317</definedName>
+    <definedName name="A2325826V_Latest">Data1!$F$317</definedName>
+    <definedName name="A2325827W">Data1!$O$1:$O$10,Data1!$O$15:$O$317</definedName>
+    <definedName name="A2325827W_Data">Data1!$O$15:$O$317</definedName>
+    <definedName name="A2325827W_Latest">Data1!$O$317</definedName>
+    <definedName name="A2325830K">Data1!$X$1:$X$10,Data1!$X$12:$X$317</definedName>
+    <definedName name="A2325830K_Data">Data1!$X$12:$X$317</definedName>
+    <definedName name="A2325830K_Latest">Data1!$X$317</definedName>
+    <definedName name="A2325831L">Data1!$G$1:$G$10,Data1!$G$11:$G$317</definedName>
+    <definedName name="A2325831L_Data">Data1!$G$11:$G$317</definedName>
+    <definedName name="A2325831L_Latest">Data1!$G$317</definedName>
+    <definedName name="A2325832R">Data1!$P$1:$P$10,Data1!$P$15:$P$317</definedName>
+    <definedName name="A2325832R_Data">Data1!$P$15:$P$317</definedName>
+    <definedName name="A2325832R_Latest">Data1!$P$317</definedName>
+    <definedName name="A2325835W">Data1!$Y$1:$Y$10,Data1!$Y$12:$Y$317</definedName>
+    <definedName name="A2325835W_Data">Data1!$Y$12:$Y$317</definedName>
+    <definedName name="A2325835W_Latest">Data1!$Y$317</definedName>
+    <definedName name="A2325836X">Data1!$H$1:$H$10,Data1!$H$139:$H$317</definedName>
+    <definedName name="A2325836X_Data">Data1!$H$139:$H$317</definedName>
+    <definedName name="A2325836X_Latest">Data1!$H$317</definedName>
+    <definedName name="A2325837A">Data1!$Q$1:$Q$10,Data1!$Q$143:$Q$317</definedName>
+    <definedName name="A2325837A_Data">Data1!$Q$143:$Q$317</definedName>
+    <definedName name="A2325837A_Latest">Data1!$Q$317</definedName>
+    <definedName name="A2325840R">Data1!$Z$1:$Z$10,Data1!$Z$140:$Z$317</definedName>
+    <definedName name="A2325840R_Data">Data1!$Z$140:$Z$317</definedName>
+    <definedName name="A2325840R_Latest">Data1!$Z$317</definedName>
+    <definedName name="A2325841T">Data1!$I$1:$I$10,Data1!$I$11:$I$317</definedName>
+    <definedName name="A2325841T_Data">Data1!$I$11:$I$317</definedName>
+    <definedName name="A2325841T_Latest">Data1!$I$317</definedName>
+    <definedName name="A2325842V">Data1!$R$1:$R$10,Data1!$R$15:$R$317</definedName>
+    <definedName name="A2325842V_Data">Data1!$R$15:$R$317</definedName>
+    <definedName name="A2325842V_Latest">Data1!$R$317</definedName>
+    <definedName name="A2325845A">Data1!$AA$1:$AA$10,Data1!$AA$12:$AA$317</definedName>
+    <definedName name="A2325845A_Data">Data1!$AA$12:$AA$317</definedName>
+    <definedName name="A2325845A_Latest">Data1!$AA$317</definedName>
+    <definedName name="A2325846C">Data1!$J$1:$J$10,Data1!$J$11:$J$317</definedName>
+    <definedName name="A2325846C_Data">Data1!$J$11:$J$317</definedName>
+    <definedName name="A2325846C_Latest">Data1!$J$317</definedName>
+    <definedName name="A2325847F">Data1!$S$1:$S$10,Data1!$S$15:$S$317</definedName>
+    <definedName name="A2325847F_Data">Data1!$S$15:$S$317</definedName>
+    <definedName name="A2325847F_Latest">Data1!$S$317</definedName>
+    <definedName name="A2325850V">Data1!$AB$1:$AB$10,Data1!$AB$12:$AB$317</definedName>
+    <definedName name="A2325850V_Data">Data1!$AB$12:$AB$317</definedName>
+    <definedName name="A2325850V_Latest">Data1!$AB$317</definedName>
+    <definedName name="Date_Range">Data1!$A$2:$A$10,Data1!$A$11:$A$317</definedName>
+    <definedName name="Date_Range_Data">Data1!$A$11:$A$317</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -629,7 +629,7 @@
     <t>Freq.</t>
   </si>
   <si>
-    <t>© Commonwealth of Australia  2024</t>
+    <t>© Commonwealth of Australia  2025</t>
   </si>
 </sst>
 </file>
@@ -1316,10 +1316,10 @@
         <v>17777</v>
       </c>
       <c r="G12" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H12" s="10">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>36</v>
@@ -1348,10 +1348,10 @@
         <v>17777</v>
       </c>
       <c r="G13" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H13" s="10">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>36</v>
@@ -1380,10 +1380,10 @@
         <v>17777</v>
       </c>
       <c r="G14" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H14" s="10">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>36</v>
@@ -1412,10 +1412,10 @@
         <v>17777</v>
       </c>
       <c r="G15" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H15" s="10">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>36</v>
@@ -1444,10 +1444,10 @@
         <v>17777</v>
       </c>
       <c r="G16" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H16" s="10">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>36</v>
@@ -1476,10 +1476,10 @@
         <v>17777</v>
       </c>
       <c r="G17" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H17" s="10">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>36</v>
@@ -1508,10 +1508,10 @@
         <v>29465</v>
       </c>
       <c r="G18" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H18" s="10">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>36</v>
@@ -1540,10 +1540,10 @@
         <v>17777</v>
       </c>
       <c r="G19" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H19" s="10">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>36</v>
@@ -1572,10 +1572,10 @@
         <v>17777</v>
       </c>
       <c r="G20" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H20" s="10">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>36</v>
@@ -1604,10 +1604,10 @@
         <v>18142</v>
       </c>
       <c r="G21" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H21" s="10">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>49</v>
@@ -1636,10 +1636,10 @@
         <v>18142</v>
       </c>
       <c r="G22" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H22" s="10">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>49</v>
@@ -1668,10 +1668,10 @@
         <v>18142</v>
       </c>
       <c r="G23" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H23" s="10">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>49</v>
@@ -1700,10 +1700,10 @@
         <v>18142</v>
       </c>
       <c r="G24" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H24" s="10">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>49</v>
@@ -1732,10 +1732,10 @@
         <v>18142</v>
       </c>
       <c r="G25" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H25" s="10">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>49</v>
@@ -1764,10 +1764,10 @@
         <v>18142</v>
       </c>
       <c r="G26" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H26" s="10">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>49</v>
@@ -1796,10 +1796,10 @@
         <v>29830</v>
       </c>
       <c r="G27" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H27" s="10">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>49</v>
@@ -1828,10 +1828,10 @@
         <v>18142</v>
       </c>
       <c r="G28" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H28" s="10">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>49</v>
@@ -1860,10 +1860,10 @@
         <v>18142</v>
       </c>
       <c r="G29" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H29" s="10">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>49</v>
@@ -1892,10 +1892,10 @@
         <v>17868</v>
       </c>
       <c r="G30" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H30" s="10">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>49</v>
@@ -1924,10 +1924,10 @@
         <v>17868</v>
       </c>
       <c r="G31" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H31" s="10">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>49</v>
@@ -1956,10 +1956,10 @@
         <v>17868</v>
       </c>
       <c r="G32" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H32" s="10">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>49</v>
@@ -1988,10 +1988,10 @@
         <v>17868</v>
       </c>
       <c r="G33" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H33" s="10">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>49</v>
@@ -2020,10 +2020,10 @@
         <v>17868</v>
       </c>
       <c r="G34" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H34" s="10">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I34" s="10" t="s">
         <v>49</v>
@@ -2052,10 +2052,10 @@
         <v>17868</v>
       </c>
       <c r="G35" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H35" s="10">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>49</v>
@@ -2084,10 +2084,10 @@
         <v>29556</v>
       </c>
       <c r="G36" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H36" s="10">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="I36" s="10" t="s">
         <v>49</v>
@@ -2116,10 +2116,10 @@
         <v>17868</v>
       </c>
       <c r="G37" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H37" s="10">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I37" s="10" t="s">
         <v>49</v>
@@ -2148,10 +2148,10 @@
         <v>17868</v>
       </c>
       <c r="G38" s="9">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H38" s="10">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>49</v>
@@ -2213,7 +2213,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB315"/>
+  <dimension ref="A1:AB317"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="10" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
@@ -2831,85 +2831,85 @@
         <v>33</v>
       </c>
       <c r="B8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="C8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="D8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="E8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="F8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="G8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="H8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="I8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="J8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="K8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="L8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="M8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="N8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="O8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="P8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="Q8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="R8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="S8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="T8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="U8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="V8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="W8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="X8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="Y8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="Z8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="AA8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
       <c r="AB8" s="6">
-        <v>45536</v>
+        <v>45717</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
@@ -2917,85 +2917,85 @@
         <v>34</v>
       </c>
       <c r="B9" s="1">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C9" s="1">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D9" s="1">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E9" s="1">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="F9" s="1">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="G9" s="1">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="H9" s="1">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="I9" s="1">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="J9" s="1">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="K9" s="1">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="L9" s="1">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="M9" s="1">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="N9" s="1">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="O9" s="1">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="P9" s="1">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="Q9" s="1">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="R9" s="1">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="S9" s="1">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="T9" s="1">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="U9" s="1">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="V9" s="1">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="W9" s="1">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="X9" s="1">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="Y9" s="1">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="Z9" s="1">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="AA9" s="1">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="AB9" s="1">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
@@ -28025,6 +28025,178 @@
       </c>
       <c r="AB315" s="8">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="316" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A316" s="9">
+        <v>45627</v>
+      </c>
+      <c r="B316" s="8">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="C316" s="8">
+        <v>139.5</v>
+      </c>
+      <c r="D316" s="8">
+        <v>140.19999999999999</v>
+      </c>
+      <c r="E316" s="8">
+        <v>140.5</v>
+      </c>
+      <c r="F316" s="8">
+        <v>137.9</v>
+      </c>
+      <c r="G316" s="8">
+        <v>138.9</v>
+      </c>
+      <c r="H316" s="8">
+        <v>133.69999999999999</v>
+      </c>
+      <c r="I316" s="8">
+        <v>137.30000000000001</v>
+      </c>
+      <c r="J316" s="8">
+        <v>139.4</v>
+      </c>
+      <c r="K316" s="8">
+        <v>2.4</v>
+      </c>
+      <c r="L316" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="M316" s="8">
+        <v>1.8</v>
+      </c>
+      <c r="N316" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="O316" s="8">
+        <v>2.9</v>
+      </c>
+      <c r="P316" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="Q316" s="8">
+        <v>1.7</v>
+      </c>
+      <c r="R316" s="8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S316" s="8">
+        <v>2.4</v>
+      </c>
+      <c r="T316" s="8">
+        <v>-0.1</v>
+      </c>
+      <c r="U316" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="V316" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="W316" s="8">
+        <v>-0.1</v>
+      </c>
+      <c r="X316" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="Y316" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="Z316" s="8">
+        <v>-0.1</v>
+      </c>
+      <c r="AA316" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="AB316" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="317" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A317" s="9">
+        <v>45717</v>
+      </c>
+      <c r="B317" s="8">
+        <v>140.9</v>
+      </c>
+      <c r="C317" s="8">
+        <v>140.69999999999999</v>
+      </c>
+      <c r="D317" s="8">
+        <v>142.9</v>
+      </c>
+      <c r="E317" s="8">
+        <v>141.19999999999999</v>
+      </c>
+      <c r="F317" s="8">
+        <v>138.6</v>
+      </c>
+      <c r="G317" s="8">
+        <v>140</v>
+      </c>
+      <c r="H317" s="8">
+        <v>134.6</v>
+      </c>
+      <c r="I317" s="8">
+        <v>138.6</v>
+      </c>
+      <c r="J317" s="8">
+        <v>140.69999999999999</v>
+      </c>
+      <c r="K317" s="8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L317" s="8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M317" s="8">
+        <v>2.7</v>
+      </c>
+      <c r="N317" s="8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O317" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="P317" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="Q317" s="8">
+        <v>1.7</v>
+      </c>
+      <c r="R317" s="8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S317" s="8">
+        <v>2.4</v>
+      </c>
+      <c r="T317" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="U317" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="V317" s="8">
+        <v>1.9</v>
+      </c>
+      <c r="W317" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="X317" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="Y317" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="Z317" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="AA317" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="AB317" s="8">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>